<commit_message>
Volunteering and certifications added
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrha\curriculum-vitae\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19D96AA-ECAC-4AE8-B6C0-1542944F0752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249BB758-F9B1-4345-AE0B-188A7ECAB9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="188">
   <si>
     <t>position</t>
   </si>
@@ -570,6 +570,52 @@
   </si>
   <si>
     <t>Management and migration of large volumes of scientific data between servers using SSH and Jupyter Server, ensuring proper organization, categorization, and accessibility. Development of an informational website on wind energy in Mexico using Quarto and Visual Studio Code, integrating data visualizations, academic publications, and educational resources. [Access the site here](https://main--eolicaierunam.netlify.app/).</t>
+  </si>
+  <si>
+    <t>Developed leadership and teamwork expertise by analyzing methods to foster individual growth and drive continuous team advancement; mastered providing and receiving feedback, conducting difficult conversations, and effectively communicating team mission, while applying trust-building and well-being strategies to enhance team performance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acquired a comprehensive foundation in leadership fundamentals within rapidly evolving technological and business environments, emphasizing the leader’s role in managing change and shaping organizational culture. Explored four dimensions of leadership (personal, team, organizational, and external) and learned practical 
+actions to inspire, connect, and mobilize teams toward effective collective action. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acquired data analysis and visualization expertise using Microsoft Power BI Desktop; connected to diverse data sources, including Excel, relational databases, and web sources like Wikipedia; shaped and transformed data with the integrated Power Query Editor; created and organized interactive visualizations and reports; and learned to publish, share, and manage Power BI assets for streamlined insight dissemination. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acquired end-to-end data analysis and business intelligence skills using the full Microsoft Power BI suite-service, Desktop, and Mobile; connected to diverse data sources, modeled and transformed data, designed and organized interactive reports, pinned and shared dashboards, employed Q&amp;A natural-language queries, and leveraged desktop data modeling capabilities for actionable insights. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acquired proficiency in Microsoft Power BI by connecting to single or multiple data sources through a secure,  intuitive interface to transform and interpret data; designing interactive dashboards and reports; collaborating seamlessly within a unified platform. </t>
+  </si>
+  <si>
+    <t>[Aprende Power BI](https://www.linkedin.com/learning/certificates/48485e6403f7f1e38136cb0bd12a35a0b1a23126e17890cbe3fee90dd7205e4b?trk=share_certificate)</t>
+  </si>
+  <si>
+    <t>[Power BI Essential Training](https://www.linkedin.com/learning/certificates/35c6e0e304e07bbd77d885270322b07eef57a3a3369d368dbda3a5848e091a70?trk=share_certificate)</t>
+  </si>
+  <si>
+    <t>[Fundamentos del liderazgo](https://www.linkedin.com/learning/certificates/fb0fb94a9866b79d5aaefac7c3bb0b04c74441320545c02b9164907700f8611a?trk=share_certificate)</t>
+  </si>
+  <si>
+    <t>[Liderazgo y trabajo en equipo](https://www.linkedin.com/learning/certificates/71801e7ea59ee135c9e4859228dc523f76c5952eb7be43184e45286c83054340?trk=share_certificate)</t>
+  </si>
+  <si>
+    <t>[Learning Power BI Desktop](https://www.linkedin.com/learning/certificates/29a74ce3989818a656bf7a9a52d13eab92825e193eddf03179d55787ed4ec8ae?trk=share_certificate)</t>
+  </si>
+  <si>
+    <t>Data Analyst and Web App Developer</t>
+  </si>
+  <si>
+    <t>IER-UNAM</t>
+  </si>
+  <si>
+    <t>Temixco, Morelos</t>
+  </si>
+  <si>
+    <t>Jul. 2025</t>
+  </si>
+  <si>
+    <t>Collaborated on the design and development of a web application for solar radiation and meteorological data monitoring and analysis (ESOLMET); gained hands-on experience in Git-based version control, Python data processing, interactive dashboard and web app development with Shiny for Python, and SQL database design and management.</t>
   </si>
 </sst>
 </file>
@@ -1674,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1705,15 +1751,15 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1721,7 +1767,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1734,10 +1780,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1745,7 +1791,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1961,10 +2007,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E050452-1706-404D-B355-6C16037B2027}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1997,23 +2043,43 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="C3" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2025,10 +2091,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25220DED-3F04-4958-9AA1-836403C9FDD5}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2198,6 +2264,106 @@
         <v>162</v>
       </c>
     </row>
+    <row r="9" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>